<commit_message>
Added Flexible Profile Admin
</commit_message>
<xml_diff>
--- a/data/testscriptdata.xlsx
+++ b/data/testscriptdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="19380" windowHeight="6435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="10485" windowHeight="3975" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A56:Q75"/>
+  <oleSize ref="A56:K66"/>
 </workbook>
 </file>
 
@@ -5288,8 +5288,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B1569"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13154,7 +13154,7 @@
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Fixed propertyPortfolioMeter Test Scripts
</commit_message>
<xml_diff>
--- a/data/testscriptdata.xlsx
+++ b/data/testscriptdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="10485" windowHeight="3975" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="14850" windowHeight="4035" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A56:K66"/>
+  <oleSize ref="A56:M67"/>
 </workbook>
 </file>
 
@@ -4838,12 +4838,6 @@
     <t>addValidHHmeterGeneric()</t>
   </si>
   <si>
-    <t>2500</t>
-  </si>
-  <si>
-    <t>3200</t>
-  </si>
-  <si>
     <t>Expected Consumption</t>
   </si>
   <si>
@@ -4865,10 +4859,16 @@
     <t>TC_14</t>
   </si>
   <si>
-    <t>2200</t>
-  </si>
-  <si>
-    <t>2800</t>
+    <t>900</t>
+  </si>
+  <si>
+    <t>950</t>
+  </si>
+  <si>
+    <t>800</t>
+  </si>
+  <si>
+    <t>850</t>
   </si>
 </sst>
 </file>
@@ -5288,8 +5288,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B1569"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="A72" sqref="A72"/>
+    <sheetView tabSelected="1" topLeftCell="A1564" workbookViewId="0">
+      <selection activeCell="C1574" sqref="C1574"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13331,10 +13331,10 @@
         <v>7</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>1608</v>
+        <v>1606</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>1609</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -13345,10 +13345,10 @@
         <v>1605</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>1606</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>1607</v>
+        <v>1613</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>1614</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -13363,21 +13363,21 @@
     </row>
     <row r="12" spans="1:12" ht="45">
       <c r="A12" s="8" t="s">
-        <v>1611</v>
+        <v>1609</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>1608</v>
+        <v>1606</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>1609</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="8" t="s">
-        <v>1612</v>
+        <v>1610</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>1610</v>
+        <v>1608</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>1615</v>
@@ -13388,12 +13388,12 @@
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="8" t="s">
-        <v>1613</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="8" t="s">
-        <v>1614</v>
+        <v>1612</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Flex management suite scripts
</commit_message>
<xml_diff>
--- a/data/testscriptdata.xlsx
+++ b/data/testscriptdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="14520" windowHeight="6435" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="15210" windowHeight="6435" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,12 +15,12 @@
     <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1:K11"/>
+  <oleSize ref="A1:O20"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1801" uniqueCount="1718">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1812" uniqueCount="1726">
   <si>
     <t>test ID</t>
   </si>
@@ -5047,9 +5047,6 @@
     <t>CustomerName</t>
   </si>
   <si>
-    <t>Auto_Company_5…</t>
-  </si>
-  <si>
     <t>MeterForeCasteForGas</t>
   </si>
   <si>
@@ -5174,6 +5171,33 @@
   </si>
   <si>
     <t>80</t>
+  </si>
+  <si>
+    <t>EON</t>
+  </si>
+  <si>
+    <t>Auto_Company_55</t>
+  </si>
+  <si>
+    <t>Tollarance</t>
+  </si>
+  <si>
+    <t>ProductName</t>
+  </si>
+  <si>
+    <t>MiniGoogle</t>
+  </si>
+  <si>
+    <t>RenewableDiscount</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>Value (£pMWh)</t>
+  </si>
+  <si>
+    <t>Supplier Clips</t>
   </si>
 </sst>
 </file>
@@ -5301,7 +5325,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -5355,6 +5379,7 @@
     <xf numFmtId="49" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -13593,7 +13618,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
@@ -13921,7 +13946,7 @@
         <v>1638</v>
       </c>
       <c r="N20" s="22" t="s">
-        <v>1716</v>
+        <v>1715</v>
       </c>
     </row>
     <row r="21" spans="2:14" ht="30">
@@ -13993,22 +14018,22 @@
     </row>
     <row r="25" spans="2:14" ht="30">
       <c r="B25" s="9" t="s">
-        <v>1712</v>
+        <v>1711</v>
       </c>
       <c r="C25" s="10" t="s">
+        <v>1713</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>1713</v>
+      </c>
+      <c r="E25" s="9" t="s">
         <v>1714</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>1714</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>1715</v>
       </c>
       <c r="F25" s="12" t="s">
         <v>1642</v>
       </c>
       <c r="G25" s="9" t="s">
-        <v>1713</v>
+        <v>1712</v>
       </c>
       <c r="J25" s="9" t="s">
         <v>1645</v>
@@ -14017,7 +14042,7 @@
         <v>1647</v>
       </c>
       <c r="N25" s="9" t="s">
-        <v>1717</v>
+        <v>1716</v>
       </c>
     </row>
   </sheetData>
@@ -14040,86 +14065,92 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:W21"/>
+  <dimension ref="A1:W27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:23">
       <c r="A1" s="18" t="s">
         <v>1673</v>
       </c>
-      <c r="B1" s="5"/>
+      <c r="B1" s="5" t="s">
+        <v>1717</v>
+      </c>
     </row>
     <row r="4" spans="1:23">
       <c r="A4" s="18" t="s">
         <v>1674</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1675</v>
+        <v>1718</v>
       </c>
     </row>
     <row r="8" spans="1:23">
       <c r="A8" s="18" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
     </row>
     <row r="9" spans="1:23">
       <c r="B9" t="s">
+        <v>1676</v>
+      </c>
+      <c r="C9" t="s">
         <v>1677</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>1678</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>1679</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>1680</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>1681</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>1682</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>1683</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>1684</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>1685</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>1686</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>1687</v>
-      </c>
-      <c r="M9" t="s">
-        <v>1688</v>
       </c>
     </row>
     <row r="10" spans="1:23">
       <c r="A10" t="s">
+        <v>1688</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>1689</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="C10" s="7" t="s">
+        <v>1689</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>1690</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="E10" s="7" t="s">
         <v>1690</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>1691</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>1691</v>
       </c>
       <c r="F10" s="7" t="s">
         <v>37</v>
@@ -14128,104 +14159,104 @@
         <v>1656</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>1692</v>
+        <v>1691</v>
       </c>
       <c r="I10" s="7" t="s">
         <v>1656</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>1693</v>
+        <v>1692</v>
       </c>
       <c r="K10" s="7" t="s">
-        <v>1691</v>
+        <v>1690</v>
       </c>
       <c r="L10" s="7" t="s">
         <v>37</v>
       </c>
       <c r="M10" s="7" t="s">
-        <v>1693</v>
+        <v>1692</v>
       </c>
     </row>
     <row r="11" spans="1:23">
       <c r="A11" t="s">
+        <v>1693</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>1694</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>1695</v>
-      </c>
       <c r="C11" s="7" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
       <c r="K11" s="7" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
       <c r="L11" s="7" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
       <c r="M11" s="7" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="12" spans="1:23">
       <c r="A12" t="s">
+        <v>1695</v>
+      </c>
+      <c r="B12" t="s">
         <v>1696</v>
       </c>
-      <c r="B12" t="s">
-        <v>1697</v>
-      </c>
       <c r="C12" t="s">
-        <v>1697</v>
+        <v>1696</v>
       </c>
       <c r="D12" t="s">
-        <v>1697</v>
+        <v>1696</v>
       </c>
       <c r="E12" t="s">
-        <v>1697</v>
+        <v>1696</v>
       </c>
       <c r="F12" t="s">
-        <v>1697</v>
+        <v>1696</v>
       </c>
       <c r="G12" t="s">
-        <v>1697</v>
+        <v>1696</v>
       </c>
       <c r="H12" t="s">
-        <v>1697</v>
+        <v>1696</v>
       </c>
       <c r="I12" t="s">
-        <v>1697</v>
+        <v>1696</v>
       </c>
       <c r="J12" t="s">
-        <v>1697</v>
+        <v>1696</v>
       </c>
       <c r="K12" t="s">
-        <v>1697</v>
+        <v>1696</v>
       </c>
       <c r="L12" t="s">
-        <v>1697</v>
+        <v>1696</v>
       </c>
       <c r="M12" t="s">
-        <v>1697</v>
+        <v>1696</v>
       </c>
     </row>
     <row r="13" spans="1:23">
@@ -14241,64 +14272,64 @@
     </row>
     <row r="14" spans="1:23">
       <c r="B14" s="18" t="s">
+        <v>1697</v>
+      </c>
+      <c r="C14" s="18" t="s">
         <v>1698</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="D14" s="18" t="s">
         <v>1699</v>
       </c>
-      <c r="D14" s="18" t="s">
+      <c r="E14" s="18" t="s">
         <v>1700</v>
       </c>
-      <c r="E14" s="18" t="s">
+      <c r="F14" s="18" t="s">
         <v>1701</v>
-      </c>
-      <c r="F14" s="18" t="s">
-        <v>1702</v>
       </c>
     </row>
     <row r="15" spans="1:23">
       <c r="A15" t="s">
+        <v>1702</v>
+      </c>
+      <c r="B15" s="19" t="s">
         <v>1703</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="C15" s="5" t="s">
         <v>1704</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="D15" s="5" t="s">
         <v>1705</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="E15" s="20" t="s">
         <v>1706</v>
       </c>
-      <c r="E15" s="20" t="s">
+      <c r="F15" s="7" t="s">
         <v>1707</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>1708</v>
       </c>
     </row>
     <row r="16" spans="1:23">
       <c r="A16" s="21" t="s">
+        <v>1708</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>1703</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>1704</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>1709</v>
       </c>
-      <c r="B16" s="19" t="s">
-        <v>1704</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>1705</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>1710</v>
-      </c>
       <c r="E16" s="20" t="s">
+        <v>1706</v>
+      </c>
+      <c r="F16" s="7" t="s">
         <v>1707</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>1708</v>
       </c>
     </row>
     <row r="20" spans="1:20">
       <c r="A20" s="18" t="s">
-        <v>1711</v>
+        <v>1710</v>
       </c>
     </row>
     <row r="21" spans="1:20">
@@ -14360,8 +14391,49 @@
         <v>10</v>
       </c>
     </row>
+    <row r="23" spans="1:20">
+      <c r="A23" t="s">
+        <v>1719</v>
+      </c>
+      <c r="B23" s="23" t="s">
+        <v>1689</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20">
+      <c r="A24" t="s">
+        <v>1720</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1721</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20">
+      <c r="A25" t="s">
+        <v>1722</v>
+      </c>
+      <c r="B25" s="23" t="s">
+        <v>1723</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20">
+      <c r="A26" t="s">
+        <v>1724</v>
+      </c>
+      <c r="B26" s="23" t="s">
+        <v>1689</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20">
+      <c r="A27" t="s">
+        <v>1725</v>
+      </c>
+      <c r="B27" s="23" t="s">
+        <v>1689</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
modified flex login details
</commit_message>
<xml_diff>
--- a/data/testscriptdata.xlsx
+++ b/data/testscriptdata.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1854" uniqueCount="1753">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1858" uniqueCount="1756">
   <si>
     <t>test ID</t>
   </si>
@@ -5281,12 +5281,22 @@
   </si>
   <si>
     <t>VACU Steel3</t>
+  </si>
+  <si>
+    <t>Smartest Energy</t>
+  </si>
+  <si>
+    <t>F&amp;S Energy</t>
+  </si>
+  <si>
+    <t>Total Gas and Power</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="7">
     <font>
       <sz val="11"/>
@@ -5775,9 +5785,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" style="2" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.42578125" style="2" customWidth="1" collapsed="1"/>
-    <col min="3" max="16384" width="9.140625" style="2" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="2" width="11.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="2" width="17.42578125" collapsed="true"/>
+    <col min="3" max="16384" style="2" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="30">
@@ -5845,7 +5855,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="29.28515625" style="5" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="5" width="29.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -13710,16 +13720,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="8" collapsed="1"/>
-    <col min="2" max="2" width="26.42578125" style="9" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.5703125" style="9" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.140625" style="9" collapsed="1"/>
-    <col min="5" max="5" width="14.7109375" style="9" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.42578125" style="9" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10.140625" style="9" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="9.140625" style="9" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="10.5703125" style="9" customWidth="1" collapsed="1"/>
-    <col min="10" max="16384" width="9.140625" style="9" collapsed="1"/>
+    <col min="1" max="1" style="8" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="9" width="26.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="9" width="12.5703125" collapsed="true"/>
+    <col min="4" max="4" style="9" width="9.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="9" width="14.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="9" width="14.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="9" width="10.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="9" width="9.140625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="9" width="10.5703125" collapsed="true"/>
+    <col min="10" max="16384" style="9" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="4" customFormat="1">
@@ -14196,10 +14206,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:5">
@@ -14246,8 +14256,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="64.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="64.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="21.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23">
@@ -14256,6 +14266,11 @@
       </c>
       <c r="B1" s="5" t="s">
         <v>1751</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="D2" t="s">
+        <v>1755</v>
       </c>
     </row>
     <row r="4" spans="1:23">
@@ -14644,13 +14659,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="14" collapsed="1"/>
-    <col min="3" max="3" width="13.140625" style="14" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25" style="14" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.85546875" style="14" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.140625" style="14" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="33.5703125" style="14" customWidth="1" collapsed="1"/>
-    <col min="8" max="16384" width="9.140625" style="14" collapsed="1"/>
+    <col min="1" max="2" style="14" width="9.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="14" width="13.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="14" width="25.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="14" width="17.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="14" width="24.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="14" width="33.5703125" collapsed="true"/>
+    <col min="8" max="16384" style="14" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="45">
@@ -14750,8 +14765,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" customWidth="1"/>
-    <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="19.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="45">

</xml_diff>

<commit_message>
Request quote error fixed
</commit_message>
<xml_diff>
--- a/data/testscriptdata.xlsx
+++ b/data/testscriptdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="15105" windowHeight="3075" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="15105" windowHeight="6435" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,12 +16,12 @@
     <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1:H20"/>
+  <oleSize ref="A1:P20"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1858" uniqueCount="1756">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1859" uniqueCount="1756">
   <si>
     <t>test ID</t>
   </si>
@@ -5283,13 +5283,13 @@
     <t>VACU Steel3</t>
   </si>
   <si>
+    <t>Total Gas and Power</t>
+  </si>
+  <si>
     <t>Smartest Energy</t>
   </si>
   <si>
     <t>F&amp;S Energy</t>
-  </si>
-  <si>
-    <t>Total Gas and Power</t>
   </si>
 </sst>
 </file>
@@ -14200,7 +14200,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -14250,7 +14250,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:W31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -14270,7 +14270,7 @@
     </row>
     <row r="2">
       <c r="D2" t="s">
-        <v>1755</v>
+        <v>1753</v>
       </c>
     </row>
     <row r="4" spans="1:23">

</xml_diff>

<commit_message>
Flex customer credentials changed
</commit_message>
<xml_diff>
--- a/data/testscriptdata.xlsx
+++ b/data/testscriptdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="19380" windowHeight="6435" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="13890" windowHeight="6435" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,12 +19,12 @@
     <sheet name="Sheet10" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1:J11"/>
+  <oleSize ref="A1:N20"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1926" uniqueCount="1787">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1930" uniqueCount="1789">
   <si>
     <t>test ID</t>
   </si>
@@ -5283,9 +5283,6 @@
     <t>EON</t>
   </si>
   <si>
-    <t>VACU Steel3</t>
-  </si>
-  <si>
     <t>Total Gas and Power</t>
   </si>
   <si>
@@ -5386,12 +5383,22 @@
   </si>
   <si>
     <t>PM_PP_TC_024</t>
+  </si>
+  <si>
+    <t>Auto_Simpro</t>
+  </si>
+  <si>
+    <t>Smartest Energy</t>
+  </si>
+  <si>
+    <t>F&amp;S Energy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="7">
     <font>
       <sz val="11"/>
@@ -5884,9 +5891,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" style="2" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.42578125" style="2" customWidth="1" collapsed="1"/>
-    <col min="3" max="16384" width="9.140625" style="2" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="2" width="11.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="2" width="17.42578125" collapsed="true"/>
+    <col min="3" max="16384" style="2" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="30">
@@ -5966,7 +5973,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="29.28515625" style="5" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="5" width="29.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -13825,22 +13832,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="8" collapsed="1"/>
-    <col min="2" max="2" width="26.42578125" style="9" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.5703125" style="9" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.140625" style="9" collapsed="1"/>
-    <col min="5" max="5" width="14.7109375" style="9" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.42578125" style="9" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10.140625" style="9" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="9.140625" style="9" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.5703125" style="9" customWidth="1" collapsed="1"/>
-    <col min="10" max="16384" width="9.140625" style="9" collapsed="1"/>
+    <col min="1" max="1" style="8" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="9" width="26.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="9" width="12.5703125" collapsed="true"/>
+    <col min="4" max="4" style="9" width="9.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="9" width="14.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="9" width="14.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="9" width="10.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="9" width="9.140625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="9" width="13.5703125" collapsed="true"/>
+    <col min="10" max="16384" style="9" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="4" customFormat="1">
@@ -14303,22 +14310,22 @@
     </row>
     <row r="34" spans="2:10" ht="60">
       <c r="C34" s="26" t="s">
+        <v>1764</v>
+      </c>
+      <c r="D34" s="26" t="s">
         <v>1765</v>
       </c>
-      <c r="D34" s="26" t="s">
+      <c r="E34" s="26" t="s">
         <v>1766</v>
       </c>
-      <c r="E34" s="26" t="s">
+      <c r="F34" s="26" t="s">
         <v>1767</v>
       </c>
-      <c r="F34" s="26" t="s">
+      <c r="G34" s="26" t="s">
         <v>1768</v>
       </c>
-      <c r="G34" s="26" t="s">
+      <c r="H34" s="26" t="s">
         <v>1769</v>
-      </c>
-      <c r="H34" s="26" t="s">
-        <v>1770</v>
       </c>
       <c r="I34" s="26" t="s">
         <v>1603</v>
@@ -14329,139 +14336,139 @@
     </row>
     <row r="35" spans="2:10">
       <c r="B35" s="9" t="s">
-        <v>1764</v>
+        <v>1763</v>
       </c>
     </row>
     <row r="36" spans="2:10">
       <c r="B36" s="9" t="s">
-        <v>1773</v>
+        <v>1772</v>
       </c>
       <c r="C36" s="10" t="s">
+        <v>1770</v>
+      </c>
+      <c r="D36" s="10" t="s">
         <v>1771</v>
-      </c>
-      <c r="D36" s="10" t="s">
-        <v>1772</v>
       </c>
     </row>
     <row r="37" spans="2:10">
       <c r="B37" s="9" t="s">
-        <v>1774</v>
+        <v>1773</v>
       </c>
       <c r="E37" s="10" t="s">
         <v>1688</v>
       </c>
       <c r="F37" s="10" t="s">
+        <v>1775</v>
+      </c>
+      <c r="G37" s="10" t="s">
         <v>1776</v>
       </c>
-      <c r="G37" s="10" t="s">
+      <c r="H37" s="10" t="s">
         <v>1777</v>
-      </c>
-      <c r="H37" s="10" t="s">
-        <v>1778</v>
       </c>
     </row>
     <row r="38" spans="2:10">
       <c r="B38" s="9" t="s">
-        <v>1775</v>
+        <v>1774</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>1772</v>
+        <v>1771</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>1779</v>
+        <v>1778</v>
       </c>
       <c r="E38" s="10" t="s">
         <v>1688</v>
       </c>
       <c r="F38" s="10" t="s">
+        <v>1775</v>
+      </c>
+      <c r="G38" s="10" t="s">
         <v>1776</v>
       </c>
-      <c r="G38" s="10" t="s">
+      <c r="H38" s="10" t="s">
         <v>1777</v>
-      </c>
-      <c r="H38" s="10" t="s">
-        <v>1778</v>
       </c>
     </row>
     <row r="39" spans="2:10">
       <c r="B39" s="9" t="s">
-        <v>1780</v>
+        <v>1779</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>1772</v>
+        <v>1771</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>1779</v>
+        <v>1778</v>
       </c>
       <c r="E39" s="10" t="s">
         <v>1688</v>
       </c>
       <c r="F39" s="10" t="s">
+        <v>1775</v>
+      </c>
+      <c r="G39" s="10" t="s">
         <v>1776</v>
       </c>
-      <c r="G39" s="10" t="s">
+      <c r="H39" s="10" t="s">
         <v>1777</v>
       </c>
-      <c r="H39" s="10" t="s">
-        <v>1778</v>
-      </c>
       <c r="I39" s="10" t="s">
-        <v>1781</v>
+        <v>1780</v>
       </c>
     </row>
     <row r="40" spans="2:10">
       <c r="B40" s="9" t="s">
-        <v>1783</v>
+        <v>1782</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>1772</v>
+        <v>1771</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>1779</v>
+        <v>1778</v>
       </c>
       <c r="E40" s="10" t="s">
         <v>1688</v>
       </c>
       <c r="F40" s="10" t="s">
+        <v>1775</v>
+      </c>
+      <c r="G40" s="10" t="s">
         <v>1776</v>
       </c>
-      <c r="G40" s="10" t="s">
+      <c r="H40" s="10" t="s">
         <v>1777</v>
       </c>
-      <c r="H40" s="10" t="s">
-        <v>1778</v>
-      </c>
       <c r="J40" s="10" t="s">
-        <v>1782</v>
+        <v>1781</v>
       </c>
     </row>
     <row r="41" spans="2:10">
       <c r="B41" s="9" t="s">
-        <v>1786</v>
+        <v>1785</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>1772</v>
+        <v>1771</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>1779</v>
+        <v>1778</v>
       </c>
       <c r="E41" s="10" t="s">
         <v>1688</v>
       </c>
       <c r="F41" s="10" t="s">
+        <v>1775</v>
+      </c>
+      <c r="G41" s="10" t="s">
         <v>1776</v>
       </c>
-      <c r="G41" s="10" t="s">
+      <c r="H41" s="10" t="s">
         <v>1777</v>
       </c>
-      <c r="H41" s="10" t="s">
-        <v>1778</v>
-      </c>
       <c r="I41" s="10" t="s">
+        <v>1783</v>
+      </c>
+      <c r="J41" s="10" t="s">
         <v>1784</v>
-      </c>
-      <c r="J41" s="10" t="s">
-        <v>1785</v>
       </c>
     </row>
   </sheetData>
@@ -14472,7 +14479,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="B1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -14480,10 +14487,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:5">
@@ -14525,13 +14532,13 @@
   <dimension ref="A1:W31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="64.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="64.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="21.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23">
@@ -14542,9 +14549,9 @@
         <v>1751</v>
       </c>
     </row>
-    <row r="2" spans="1:23">
+    <row r="2">
       <c r="D2" t="s">
-        <v>1753</v>
+        <v>1752</v>
       </c>
     </row>
     <row r="4" spans="1:23">
@@ -14552,7 +14559,7 @@
         <v>1673</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1752</v>
+        <v>1786</v>
       </c>
     </row>
     <row r="8" spans="1:23">
@@ -14933,13 +14940,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="14" collapsed="1"/>
-    <col min="3" max="3" width="13.140625" style="14" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25" style="14" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.85546875" style="14" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.140625" style="14" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="33.5703125" style="14" customWidth="1" collapsed="1"/>
-    <col min="8" max="16384" width="9.140625" style="14" collapsed="1"/>
+    <col min="1" max="2" style="14" width="9.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="14" width="13.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="14" width="25.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="14" width="17.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="14" width="24.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="14" width="33.5703125" collapsed="true"/>
+    <col min="8" max="16384" style="14" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="45">
@@ -15039,13 +15046,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.140625" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.28515625" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="16.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="13.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="30">
@@ -15103,22 +15110,22 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>1754</v>
+        <v>1753</v>
       </c>
       <c r="C7" s="18" t="s">
         <v>1654</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>1755</v>
+        <v>1754</v>
       </c>
       <c r="E7" s="18" t="s">
         <v>1665</v>
       </c>
       <c r="F7" s="18" t="s">
+        <v>1757</v>
+      </c>
+      <c r="G7" s="18" t="s">
         <v>1758</v>
-      </c>
-      <c r="G7" s="18" t="s">
-        <v>1759</v>
       </c>
       <c r="H7" s="18" t="s">
         <v>1658</v>
@@ -15130,13 +15137,13 @@
         <v>1688</v>
       </c>
       <c r="D8" t="s">
+        <v>1755</v>
+      </c>
+      <c r="E8" t="s">
         <v>1756</v>
       </c>
-      <c r="E8" t="s">
-        <v>1757</v>
-      </c>
       <c r="F8" s="25" t="s">
-        <v>1760</v>
+        <v>1759</v>
       </c>
       <c r="G8" t="s">
         <v>1650</v>
@@ -15147,7 +15154,7 @@
     </row>
     <row r="10" spans="1:12">
       <c r="B10" t="s">
-        <v>1761</v>
+        <v>1760</v>
       </c>
       <c r="C10" s="18" t="s">
         <v>1633</v>
@@ -15164,13 +15171,13 @@
     </row>
     <row r="11" spans="1:12">
       <c r="C11" s="23" t="s">
-        <v>1762</v>
+        <v>1761</v>
       </c>
       <c r="D11" s="23" t="s">
         <v>1688</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>1763</v>
+        <v>1762</v>
       </c>
       <c r="F11" s="23" t="s">
         <v>23</v>
@@ -15186,7 +15193,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>

</xml_diff>

<commit_message>
Forcasting and Manage Tender Tests added
</commit_message>
<xml_diff>
--- a/data/testscriptdata.xlsx
+++ b/data/testscriptdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="13890" windowHeight="6435" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="13890" windowHeight="4620" firstSheet="2" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,12 +19,12 @@
     <sheet name="Sheet10" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1:N20"/>
+  <oleSize ref="A1:N14"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1930" uniqueCount="1789">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1940" uniqueCount="1798">
   <si>
     <t>test ID</t>
   </si>
@@ -5388,17 +5388,43 @@
     <t>Auto_Simpro</t>
   </si>
   <si>
-    <t>Smartest Energy</t>
-  </si>
-  <si>
-    <t>F&amp;S Energy</t>
+    <t>Request Quote Link</t>
+  </si>
+  <si>
+    <t>/Quote/RequestQuote</t>
+  </si>
+  <si>
+    <t>Manage Tenders</t>
+  </si>
+  <si>
+    <t>/ManageTenders</t>
+  </si>
+  <si>
+    <t>AddBudget%</t>
+  </si>
+  <si>
+    <t>AddRaising%</t>
+  </si>
+  <si>
+    <t>Falling%</t>
+  </si>
+  <si>
+    <t>ContractYearForAnalysis</t>
+  </si>
+  <si>
+    <t>Projected Cost</t>
+  </si>
+  <si>
+    <t>2011</t>
+  </si>
+  <si>
+    <t>2012</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="7">
     <font>
       <sz val="11"/>
@@ -5891,9 +5917,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="11.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="2" width="17.42578125" collapsed="true"/>
-    <col min="3" max="16384" style="2" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="11.85546875" style="2" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.42578125" style="2" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.140625" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="30">
@@ -5973,7 +5999,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="5" width="29.28515625" collapsed="true"/>
+    <col min="1" max="1" width="29.28515625" style="5" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -13838,16 +13864,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" style="8" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="9" width="26.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="9" width="12.5703125" collapsed="true"/>
-    <col min="4" max="4" style="9" width="9.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="9" width="14.7109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="9" width="14.42578125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="9" width="10.140625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="9" width="9.140625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="9" width="13.5703125" collapsed="true"/>
-    <col min="10" max="16384" style="9" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="8" collapsed="1"/>
+    <col min="2" max="2" width="26.42578125" style="9" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.5703125" style="9" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.140625" style="9" collapsed="1"/>
+    <col min="5" max="5" width="14.7109375" style="9" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.42578125" style="9" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="10.140625" style="9" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="9.140625" style="9" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.5703125" style="9" customWidth="1" collapsed="1"/>
+    <col min="10" max="16384" width="9.140625" style="9" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="4" customFormat="1">
@@ -14479,21 +14505,23 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:E2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="19.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="1" max="1" width="18" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="21.140625" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5">
+    <row r="1" spans="2:8">
       <c r="B1" s="18" t="s">
         <v>1610</v>
       </c>
@@ -14506,8 +14534,14 @@
       <c r="E1" s="18" t="s">
         <v>1728</v>
       </c>
-    </row>
-    <row r="2" spans="2:5">
+      <c r="G1" s="18" t="s">
+        <v>1787</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>1789</v>
+      </c>
+    </row>
+    <row r="2" spans="2:8">
       <c r="B2" t="s">
         <v>1733</v>
       </c>
@@ -14519,6 +14553,12 @@
       </c>
       <c r="E2" s="7" t="s">
         <v>1566</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1788</v>
+      </c>
+      <c r="H2" t="s">
+        <v>1790</v>
       </c>
     </row>
   </sheetData>
@@ -14537,8 +14577,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="64.42578125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="21.28515625" collapsed="true"/>
+    <col min="1" max="1" width="64.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23">
@@ -14549,7 +14589,7 @@
         <v>1751</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:23">
       <c r="D2" t="s">
         <v>1752</v>
       </c>
@@ -14940,13 +14980,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" style="14" width="9.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="14" width="13.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="14" width="25.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="14" width="17.85546875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="14" width="24.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="14" width="33.5703125" collapsed="true"/>
-    <col min="8" max="16384" style="14" width="9.140625" collapsed="true"/>
+    <col min="1" max="2" width="9.140625" style="14" collapsed="1"/>
+    <col min="3" max="3" width="13.140625" style="14" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25" style="14" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.85546875" style="14" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="24.140625" style="14" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="33.5703125" style="14" customWidth="1" collapsed="1"/>
+    <col min="8" max="16384" width="9.140625" style="14" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="45">
@@ -15046,13 +15086,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="17.42578125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="12.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="16.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="17.28515625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="13.5703125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="1" max="1" width="17.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="13.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="30">
@@ -15191,26 +15231,72 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A4:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>1688</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>1792</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>1688</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>1793</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>1688</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="B1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="2:3">
+      <c r="B1" t="s">
+        <v>1794</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1795</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3">
+      <c r="B3" s="23" t="s">
+        <v>1796</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3">
+      <c r="B4" s="23" t="s">
+        <v>1797</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
modified flex account details
</commit_message>
<xml_diff>
--- a/data/testscriptdata.xlsx
+++ b/data/testscriptdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="13890" windowHeight="4620" firstSheet="2" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="13890" windowHeight="6435" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Sheet10" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1:N14"/>
+  <oleSize ref="A1:H20"/>
 </workbook>
 </file>
 
@@ -5385,9 +5385,6 @@
     <t>PM_PP_TC_024</t>
   </si>
   <si>
-    <t>Auto_Simpro</t>
-  </si>
-  <si>
     <t>Request Quote Link</t>
   </si>
   <si>
@@ -5419,6 +5416,9 @@
   </si>
   <si>
     <t>2012</t>
+  </si>
+  <si>
+    <t>VACU Steel3</t>
   </si>
 </sst>
 </file>
@@ -14507,7 +14507,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -14535,10 +14535,10 @@
         <v>1728</v>
       </c>
       <c r="G1" s="18" t="s">
-        <v>1787</v>
+        <v>1786</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>1789</v>
+        <v>1788</v>
       </c>
     </row>
     <row r="2" spans="2:8">
@@ -14555,10 +14555,10 @@
         <v>1566</v>
       </c>
       <c r="G2" t="s">
-        <v>1788</v>
+        <v>1787</v>
       </c>
       <c r="H2" t="s">
-        <v>1790</v>
+        <v>1789</v>
       </c>
     </row>
   </sheetData>
@@ -14572,7 +14572,7 @@
   <dimension ref="A1:W31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14599,7 +14599,7 @@
         <v>1673</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1786</v>
+        <v>1797</v>
       </c>
     </row>
     <row r="8" spans="1:23">
@@ -15241,7 +15241,7 @@
   <sheetData>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>1791</v>
+        <v>1790</v>
       </c>
       <c r="B4" s="23" t="s">
         <v>1688</v>
@@ -15249,7 +15249,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>1792</v>
+        <v>1791</v>
       </c>
       <c r="B5" s="23" t="s">
         <v>1688</v>
@@ -15257,7 +15257,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>1793</v>
+        <v>1792</v>
       </c>
       <c r="B6" s="23" t="s">
         <v>1688</v>
@@ -15272,7 +15272,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -15280,20 +15280,20 @@
   <sheetData>
     <row r="1" spans="2:3">
       <c r="B1" t="s">
+        <v>1793</v>
+      </c>
+      <c r="C1" t="s">
         <v>1794</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1795</v>
       </c>
     </row>
     <row r="3" spans="2:3">
       <c r="B3" s="23" t="s">
-        <v>1796</v>
+        <v>1795</v>
       </c>
     </row>
     <row r="4" spans="2:3">
       <c r="B4" s="23" t="s">
-        <v>1797</v>
+        <v>1796</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Gas suite error fixed
</commit_message>
<xml_diff>
--- a/data/testscriptdata.xlsx
+++ b/data/testscriptdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="13890" windowHeight="6435" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="14880" windowHeight="4215" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,12 +19,12 @@
     <sheet name="Sheet10" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1:H20"/>
+  <oleSize ref="E1:N8"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1940" uniqueCount="1798">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1945" uniqueCount="1803">
   <si>
     <t>test ID</t>
   </si>
@@ -5028,9 +5028,6 @@
   </si>
   <si>
     <t>Upload Price</t>
-  </si>
-  <si>
-    <t>C:\\Users\\prasanna\\Desktop\\OEM_Excel\\Testing.docx</t>
   </si>
   <si>
     <t>addValidNHHcontractHistory()</t>
@@ -5419,6 +5416,24 @@
   </si>
   <si>
     <t>VACU Steel3</t>
+  </si>
+  <si>
+    <t>14/11/2019</t>
+  </si>
+  <si>
+    <t>VACU Steel3, OEM01869, 24 (HH), EON (MiniGoogle) - (14/11/2019 08:33)</t>
+  </si>
+  <si>
+    <t>4444444444</t>
+  </si>
+  <si>
+    <t>Gas</t>
+  </si>
+  <si>
+    <t>NHH</t>
+  </si>
+  <si>
+    <t>C:\\Users\\prasanna\\Desktop\\OEM_Excel\\PriceUpload_Gas.xlsx</t>
   </si>
 </sst>
 </file>
@@ -13858,8 +13873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I40" sqref="I40"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14186,7 +14201,7 @@
         <v>1638</v>
       </c>
       <c r="N20" s="22" t="s">
-        <v>1714</v>
+        <v>1713</v>
       </c>
     </row>
     <row r="21" spans="2:14" ht="30">
@@ -14226,16 +14241,16 @@
     </row>
     <row r="23" spans="2:14" ht="30">
       <c r="B23" s="9" t="s">
+        <v>1668</v>
+      </c>
+      <c r="C23" s="10" t="s">
         <v>1669</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="D23" s="9" t="s">
+        <v>1669</v>
+      </c>
+      <c r="E23" s="9" t="s">
         <v>1670</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>1670</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>1671</v>
       </c>
       <c r="F23" s="12" t="s">
         <v>1642</v>
@@ -14258,22 +14273,22 @@
     </row>
     <row r="25" spans="2:14" ht="30">
       <c r="B25" s="9" t="s">
-        <v>1710</v>
+        <v>1709</v>
       </c>
       <c r="C25" s="10" t="s">
+        <v>1711</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>1711</v>
+      </c>
+      <c r="E25" s="9" t="s">
         <v>1712</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>1712</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>1713</v>
       </c>
       <c r="F25" s="12" t="s">
         <v>1642</v>
       </c>
       <c r="G25" s="9" t="s">
-        <v>1711</v>
+        <v>1710</v>
       </c>
       <c r="J25" s="9" t="s">
         <v>1645</v>
@@ -14282,76 +14297,76 @@
         <v>1647</v>
       </c>
       <c r="N25" s="9" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
     </row>
     <row r="28" spans="2:14" ht="45">
       <c r="B28" s="9" t="s">
-        <v>1746</v>
+        <v>1745</v>
       </c>
     </row>
     <row r="29" spans="2:14">
       <c r="B29" s="9" t="s">
-        <v>1747</v>
+        <v>1746</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
       <c r="H29" s="9" t="s">
-        <v>1738</v>
+        <v>1737</v>
       </c>
     </row>
     <row r="30" spans="2:14">
       <c r="B30" s="9" t="s">
-        <v>1748</v>
+        <v>1747</v>
       </c>
       <c r="C30" s="9" t="s">
+        <v>1738</v>
+      </c>
+      <c r="I30" s="9" t="s">
         <v>1739</v>
-      </c>
-      <c r="I30" s="9" t="s">
-        <v>1740</v>
       </c>
     </row>
     <row r="31" spans="2:14">
       <c r="B31" s="9" t="s">
-        <v>1749</v>
+        <v>1748</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>1743</v>
+        <v>1742</v>
       </c>
       <c r="J31" s="9" t="s">
-        <v>1741</v>
+        <v>1740</v>
       </c>
     </row>
     <row r="32" spans="2:14">
       <c r="B32" s="9" t="s">
-        <v>1750</v>
+        <v>1749</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>1744</v>
+        <v>1743</v>
       </c>
       <c r="K32" s="9" t="s">
-        <v>1742</v>
+        <v>1741</v>
       </c>
     </row>
     <row r="34" spans="2:10" ht="60">
       <c r="C34" s="26" t="s">
+        <v>1763</v>
+      </c>
+      <c r="D34" s="26" t="s">
         <v>1764</v>
       </c>
-      <c r="D34" s="26" t="s">
+      <c r="E34" s="26" t="s">
         <v>1765</v>
       </c>
-      <c r="E34" s="26" t="s">
+      <c r="F34" s="26" t="s">
         <v>1766</v>
       </c>
-      <c r="F34" s="26" t="s">
+      <c r="G34" s="26" t="s">
         <v>1767</v>
       </c>
-      <c r="G34" s="26" t="s">
+      <c r="H34" s="26" t="s">
         <v>1768</v>
-      </c>
-      <c r="H34" s="26" t="s">
-        <v>1769</v>
       </c>
       <c r="I34" s="26" t="s">
         <v>1603</v>
@@ -14362,139 +14377,139 @@
     </row>
     <row r="35" spans="2:10">
       <c r="B35" s="9" t="s">
-        <v>1763</v>
+        <v>1762</v>
       </c>
     </row>
     <row r="36" spans="2:10">
       <c r="B36" s="9" t="s">
-        <v>1772</v>
+        <v>1771</v>
       </c>
       <c r="C36" s="10" t="s">
+        <v>1769</v>
+      </c>
+      <c r="D36" s="10" t="s">
         <v>1770</v>
-      </c>
-      <c r="D36" s="10" t="s">
-        <v>1771</v>
       </c>
     </row>
     <row r="37" spans="2:10">
       <c r="B37" s="9" t="s">
-        <v>1773</v>
+        <v>1772</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>1688</v>
+        <v>1687</v>
       </c>
       <c r="F37" s="10" t="s">
+        <v>1774</v>
+      </c>
+      <c r="G37" s="10" t="s">
         <v>1775</v>
       </c>
-      <c r="G37" s="10" t="s">
+      <c r="H37" s="10" t="s">
         <v>1776</v>
-      </c>
-      <c r="H37" s="10" t="s">
-        <v>1777</v>
       </c>
     </row>
     <row r="38" spans="2:10">
       <c r="B38" s="9" t="s">
+        <v>1773</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>1770</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>1777</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>1687</v>
+      </c>
+      <c r="F38" s="10" t="s">
         <v>1774</v>
       </c>
-      <c r="C38" s="9" t="s">
-        <v>1771</v>
-      </c>
-      <c r="D38" s="9" t="s">
-        <v>1778</v>
-      </c>
-      <c r="E38" s="10" t="s">
-        <v>1688</v>
-      </c>
-      <c r="F38" s="10" t="s">
+      <c r="G38" s="10" t="s">
         <v>1775</v>
       </c>
-      <c r="G38" s="10" t="s">
+      <c r="H38" s="10" t="s">
         <v>1776</v>
-      </c>
-      <c r="H38" s="10" t="s">
-        <v>1777</v>
       </c>
     </row>
     <row r="39" spans="2:10">
       <c r="B39" s="9" t="s">
+        <v>1778</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>1770</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>1777</v>
+      </c>
+      <c r="E39" s="10" t="s">
+        <v>1687</v>
+      </c>
+      <c r="F39" s="10" t="s">
+        <v>1774</v>
+      </c>
+      <c r="G39" s="10" t="s">
+        <v>1775</v>
+      </c>
+      <c r="H39" s="10" t="s">
+        <v>1776</v>
+      </c>
+      <c r="I39" s="10" t="s">
         <v>1779</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>1771</v>
-      </c>
-      <c r="D39" s="9" t="s">
-        <v>1778</v>
-      </c>
-      <c r="E39" s="10" t="s">
-        <v>1688</v>
-      </c>
-      <c r="F39" s="10" t="s">
-        <v>1775</v>
-      </c>
-      <c r="G39" s="10" t="s">
-        <v>1776</v>
-      </c>
-      <c r="H39" s="10" t="s">
-        <v>1777</v>
-      </c>
-      <c r="I39" s="10" t="s">
-        <v>1780</v>
       </c>
     </row>
     <row r="40" spans="2:10">
       <c r="B40" s="9" t="s">
-        <v>1782</v>
+        <v>1781</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>1771</v>
+        <v>1770</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>1778</v>
+        <v>1777</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>1688</v>
+        <v>1687</v>
       </c>
       <c r="F40" s="10" t="s">
+        <v>1774</v>
+      </c>
+      <c r="G40" s="10" t="s">
         <v>1775</v>
       </c>
-      <c r="G40" s="10" t="s">
+      <c r="H40" s="10" t="s">
         <v>1776</v>
       </c>
-      <c r="H40" s="10" t="s">
-        <v>1777</v>
-      </c>
       <c r="J40" s="10" t="s">
-        <v>1781</v>
+        <v>1780</v>
       </c>
     </row>
     <row r="41" spans="2:10">
       <c r="B41" s="9" t="s">
-        <v>1785</v>
+        <v>1784</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>1771</v>
+        <v>1770</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>1778</v>
+        <v>1777</v>
       </c>
       <c r="E41" s="10" t="s">
-        <v>1688</v>
+        <v>1687</v>
       </c>
       <c r="F41" s="10" t="s">
+        <v>1774</v>
+      </c>
+      <c r="G41" s="10" t="s">
         <v>1775</v>
       </c>
-      <c r="G41" s="10" t="s">
+      <c r="H41" s="10" t="s">
         <v>1776</v>
       </c>
-      <c r="H41" s="10" t="s">
-        <v>1777</v>
-      </c>
       <c r="I41" s="10" t="s">
+        <v>1782</v>
+      </c>
+      <c r="J41" s="10" t="s">
         <v>1783</v>
-      </c>
-      <c r="J41" s="10" t="s">
-        <v>1784</v>
       </c>
     </row>
   </sheetData>
@@ -14505,10 +14520,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14517,8 +14532,8 @@
     <col min="2" max="2" width="19.85546875" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="12.85546875" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="15.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="21.140625" customWidth="1"/>
-    <col min="8" max="8" width="16.5703125" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="16.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8">
@@ -14526,39 +14541,52 @@
         <v>1610</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>1723</v>
+        <v>1722</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>1725</v>
+        <v>1724</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>1728</v>
+        <v>1727</v>
       </c>
       <c r="G1" s="18" t="s">
-        <v>1786</v>
+        <v>1785</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>1788</v>
+        <v>1787</v>
       </c>
     </row>
     <row r="2" spans="2:8">
       <c r="B2" t="s">
-        <v>1733</v>
+        <v>1732</v>
       </c>
       <c r="C2" t="s">
-        <v>1724</v>
+        <v>1723</v>
       </c>
       <c r="D2" t="s">
-        <v>1726</v>
+        <v>1725</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>1566</v>
       </c>
       <c r="G2" t="s">
-        <v>1787</v>
+        <v>1786</v>
       </c>
       <c r="H2" t="s">
-        <v>1789</v>
+        <v>1788</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8">
+      <c r="D3" t="s">
+        <v>1801</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>1799</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8">
+      <c r="D4" t="s">
+        <v>1800</v>
       </c>
     </row>
   </sheetData>
@@ -14583,83 +14611,83 @@
   <sheetData>
     <row r="1" spans="1:23">
       <c r="A1" s="18" t="s">
-        <v>1672</v>
+        <v>1671</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>1751</v>
+        <v>1750</v>
       </c>
     </row>
     <row r="2" spans="1:23">
       <c r="D2" t="s">
-        <v>1752</v>
+        <v>1751</v>
       </c>
     </row>
     <row r="4" spans="1:23">
       <c r="A4" s="18" t="s">
-        <v>1673</v>
+        <v>1672</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1797</v>
+        <v>1796</v>
       </c>
     </row>
     <row r="8" spans="1:23">
       <c r="A8" s="18" t="s">
-        <v>1674</v>
+        <v>1673</v>
       </c>
     </row>
     <row r="9" spans="1:23">
       <c r="B9" t="s">
+        <v>1674</v>
+      </c>
+      <c r="C9" t="s">
         <v>1675</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>1676</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>1677</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>1678</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>1679</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>1680</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>1681</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>1682</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>1683</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>1684</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>1685</v>
-      </c>
-      <c r="M9" t="s">
-        <v>1686</v>
       </c>
     </row>
     <row r="10" spans="1:23">
       <c r="A10" t="s">
+        <v>1686</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>1687</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="C10" s="7" t="s">
+        <v>1687</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>1688</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="E10" s="7" t="s">
         <v>1688</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>1689</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>1689</v>
       </c>
       <c r="F10" s="7" t="s">
         <v>37</v>
@@ -14668,104 +14696,104 @@
         <v>1656</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>1690</v>
+        <v>1689</v>
       </c>
       <c r="I10" s="7" t="s">
         <v>1656</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>1691</v>
+        <v>1690</v>
       </c>
       <c r="K10" s="7" t="s">
-        <v>1689</v>
+        <v>1688</v>
       </c>
       <c r="L10" s="7" t="s">
         <v>37</v>
       </c>
       <c r="M10" s="7" t="s">
-        <v>1691</v>
+        <v>1690</v>
       </c>
     </row>
     <row r="11" spans="1:23">
       <c r="A11" t="s">
+        <v>1691</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>1692</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>1693</v>
-      </c>
       <c r="C11" s="7" t="s">
-        <v>1693</v>
+        <v>1692</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>1693</v>
+        <v>1692</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>1693</v>
+        <v>1692</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>1693</v>
+        <v>1692</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>1693</v>
+        <v>1692</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>1693</v>
+        <v>1692</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>1693</v>
+        <v>1692</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>1693</v>
+        <v>1692</v>
       </c>
       <c r="K11" s="7" t="s">
-        <v>1693</v>
+        <v>1692</v>
       </c>
       <c r="L11" s="7" t="s">
-        <v>1693</v>
+        <v>1692</v>
       </c>
       <c r="M11" s="7" t="s">
-        <v>1693</v>
+        <v>1692</v>
       </c>
     </row>
     <row r="12" spans="1:23">
       <c r="A12" t="s">
+        <v>1693</v>
+      </c>
+      <c r="B12" t="s">
         <v>1694</v>
       </c>
-      <c r="B12" t="s">
-        <v>1695</v>
-      </c>
       <c r="C12" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
       <c r="D12" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
       <c r="E12" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
       <c r="F12" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
       <c r="G12" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
       <c r="H12" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
       <c r="I12" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
       <c r="J12" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
       <c r="K12" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
       <c r="L12" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
       <c r="M12" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="13" spans="1:23">
@@ -14781,64 +14809,64 @@
     </row>
     <row r="14" spans="1:23">
       <c r="B14" s="18" t="s">
+        <v>1695</v>
+      </c>
+      <c r="C14" s="18" t="s">
         <v>1696</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="D14" s="18" t="s">
         <v>1697</v>
       </c>
-      <c r="D14" s="18" t="s">
+      <c r="E14" s="18" t="s">
         <v>1698</v>
       </c>
-      <c r="E14" s="18" t="s">
+      <c r="F14" s="18" t="s">
         <v>1699</v>
-      </c>
-      <c r="F14" s="18" t="s">
-        <v>1700</v>
       </c>
     </row>
     <row r="15" spans="1:23">
       <c r="A15" t="s">
+        <v>1700</v>
+      </c>
+      <c r="B15" s="19" t="s">
         <v>1701</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="C15" s="5" t="s">
         <v>1702</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="D15" s="5" t="s">
         <v>1703</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="E15" s="20" t="s">
         <v>1704</v>
       </c>
-      <c r="E15" s="20" t="s">
+      <c r="F15" s="7" t="s">
         <v>1705</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>1706</v>
       </c>
     </row>
     <row r="16" spans="1:23">
       <c r="A16" s="21" t="s">
+        <v>1706</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>1701</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>1702</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>1707</v>
       </c>
-      <c r="B16" s="19" t="s">
-        <v>1702</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>1703</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>1708</v>
-      </c>
       <c r="E16" s="20" t="s">
+        <v>1704</v>
+      </c>
+      <c r="F16" s="7" t="s">
         <v>1705</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>1706</v>
       </c>
     </row>
     <row r="20" spans="1:20">
       <c r="A20" s="18" t="s">
-        <v>1709</v>
+        <v>1708</v>
       </c>
     </row>
     <row r="21" spans="1:20">
@@ -14902,63 +14930,63 @@
     </row>
     <row r="23" spans="1:20">
       <c r="A23" t="s">
-        <v>1716</v>
+        <v>1715</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>1688</v>
+        <v>1687</v>
       </c>
     </row>
     <row r="24" spans="1:20">
       <c r="A24" t="s">
+        <v>1716</v>
+      </c>
+      <c r="B24" t="s">
         <v>1717</v>
-      </c>
-      <c r="B24" t="s">
-        <v>1718</v>
       </c>
     </row>
     <row r="25" spans="1:20">
       <c r="A25" t="s">
+        <v>1718</v>
+      </c>
+      <c r="B25" s="23" t="s">
         <v>1719</v>
-      </c>
-      <c r="B25" s="23" t="s">
-        <v>1720</v>
       </c>
     </row>
     <row r="26" spans="1:20">
       <c r="A26" t="s">
-        <v>1721</v>
+        <v>1720</v>
       </c>
       <c r="B26" s="23" t="s">
-        <v>1688</v>
+        <v>1687</v>
       </c>
     </row>
     <row r="27" spans="1:20">
       <c r="A27" t="s">
-        <v>1722</v>
+        <v>1721</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>1688</v>
+        <v>1687</v>
       </c>
     </row>
     <row r="29" spans="1:20" ht="30">
       <c r="A29" s="2" t="s">
-        <v>1729</v>
+        <v>1728</v>
       </c>
       <c r="B29" s="23" t="s">
-        <v>1688</v>
+        <v>1687</v>
       </c>
     </row>
     <row r="30" spans="1:20">
       <c r="A30" t="s">
+        <v>1729</v>
+      </c>
+      <c r="B30" s="23" t="s">
         <v>1730</v>
-      </c>
-      <c r="B30" s="23" t="s">
-        <v>1731</v>
       </c>
     </row>
     <row r="31" spans="1:20">
       <c r="A31" t="s">
-        <v>1732</v>
+        <v>1731</v>
       </c>
       <c r="B31" s="23" t="s">
         <v>1644</v>
@@ -14974,8 +15002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -15041,7 +15069,7 @@
         <v>1666</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>1727</v>
+        <v>1726</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="30">
@@ -15052,7 +15080,7 @@
         <v>1650</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>1668</v>
+        <v>1802</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -15097,13 +15125,13 @@
   <sheetData>
     <row r="1" spans="1:12" ht="30">
       <c r="A1" t="s">
-        <v>1734</v>
+        <v>1733</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>1735</v>
+        <v>1734</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>12</v>
@@ -15140,32 +15168,32 @@
     </row>
     <row r="3" spans="1:12">
       <c r="C3" s="23" t="s">
-        <v>1736</v>
+        <v>1735</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="C4" s="23" t="s">
-        <v>1737</v>
+        <v>1736</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>1753</v>
+        <v>1752</v>
       </c>
       <c r="C7" s="18" t="s">
         <v>1654</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>1754</v>
+        <v>1753</v>
       </c>
       <c r="E7" s="18" t="s">
         <v>1665</v>
       </c>
       <c r="F7" s="18" t="s">
+        <v>1756</v>
+      </c>
+      <c r="G7" s="18" t="s">
         <v>1757</v>
-      </c>
-      <c r="G7" s="18" t="s">
-        <v>1758</v>
       </c>
       <c r="H7" s="18" t="s">
         <v>1658</v>
@@ -15174,16 +15202,16 @@
     </row>
     <row r="8" spans="1:12">
       <c r="C8" s="23" t="s">
-        <v>1688</v>
+        <v>1687</v>
       </c>
       <c r="D8" t="s">
+        <v>1754</v>
+      </c>
+      <c r="E8" t="s">
         <v>1755</v>
       </c>
-      <c r="E8" t="s">
-        <v>1756</v>
-      </c>
       <c r="F8" s="25" t="s">
-        <v>1759</v>
+        <v>1758</v>
       </c>
       <c r="G8" t="s">
         <v>1650</v>
@@ -15194,7 +15222,7 @@
     </row>
     <row r="10" spans="1:12">
       <c r="B10" t="s">
-        <v>1760</v>
+        <v>1759</v>
       </c>
       <c r="C10" s="18" t="s">
         <v>1633</v>
@@ -15211,13 +15239,13 @@
     </row>
     <row r="11" spans="1:12">
       <c r="C11" s="23" t="s">
+        <v>1760</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>1687</v>
+      </c>
+      <c r="E11" s="23" t="s">
         <v>1761</v>
-      </c>
-      <c r="D11" s="23" t="s">
-        <v>1688</v>
-      </c>
-      <c r="E11" s="23" t="s">
-        <v>1762</v>
       </c>
       <c r="F11" s="23" t="s">
         <v>23</v>
@@ -15231,7 +15259,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A4:B6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
@@ -15239,28 +15267,38 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="4" spans="1:2">
+    <row r="1" spans="1:3">
+      <c r="C1" t="s">
+        <v>1798</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>1797</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
+        <v>1789</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>1687</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
         <v>1790</v>
       </c>
-      <c r="B4" s="23" t="s">
-        <v>1688</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
+      <c r="B5" s="23" t="s">
+        <v>1687</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
         <v>1791</v>
       </c>
-      <c r="B5" s="23" t="s">
-        <v>1688</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>1792</v>
-      </c>
       <c r="B6" s="23" t="s">
-        <v>1688</v>
+        <v>1687</v>
       </c>
     </row>
   </sheetData>
@@ -15280,20 +15318,20 @@
   <sheetData>
     <row r="1" spans="2:3">
       <c r="B1" t="s">
+        <v>1792</v>
+      </c>
+      <c r="C1" t="s">
         <v>1793</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1794</v>
       </c>
     </row>
     <row r="3" spans="2:3">
       <c r="B3" s="23" t="s">
-        <v>1795</v>
+        <v>1794</v>
       </c>
     </row>
     <row r="4" spans="2:3">
       <c r="B4" s="23" t="s">
-        <v>1796</v>
+        <v>1795</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified tenders and alerts
</commit_message>
<xml_diff>
--- a/data/testscriptdata.xlsx
+++ b/data/testscriptdata.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1945" uniqueCount="1803">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1959" uniqueCount="1807">
   <si>
     <t>test ID</t>
   </si>
@@ -5434,12 +5434,25 @@
   </si>
   <si>
     <t>C:\\Users\\prasanna\\Desktop\\OEM_Excel\\PriceUpload_Gas.xlsx</t>
+  </si>
+  <si>
+    <t>Smartest Energy</t>
+  </si>
+  <si>
+    <t>F&amp;S Energy</t>
+  </si>
+  <si>
+    <t>16/11/2019</t>
+  </si>
+  <si>
+    <t>VACU Steel3, OEM01875, 24 (HH), EON (MiniGoogle) - (16/11/2019 07:50)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="7">
     <font>
       <sz val="11"/>
@@ -5932,9 +5945,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" style="2" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.42578125" style="2" customWidth="1" collapsed="1"/>
-    <col min="3" max="16384" width="9.140625" style="2" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="2" width="11.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="2" width="17.42578125" collapsed="true"/>
+    <col min="3" max="16384" style="2" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="30">
@@ -6014,7 +6027,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="29.28515625" style="5" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="5" width="29.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -13879,16 +13892,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="8" collapsed="1"/>
-    <col min="2" max="2" width="26.42578125" style="9" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.5703125" style="9" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.140625" style="9" collapsed="1"/>
-    <col min="5" max="5" width="14.7109375" style="9" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.42578125" style="9" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10.140625" style="9" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="9.140625" style="9" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.5703125" style="9" customWidth="1" collapsed="1"/>
-    <col min="10" max="16384" width="9.140625" style="9" collapsed="1"/>
+    <col min="1" max="1" style="8" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="9" width="26.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="9" width="12.5703125" collapsed="true"/>
+    <col min="4" max="4" style="9" width="9.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="9" width="14.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="9" width="14.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="9" width="10.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="9" width="9.140625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="9" width="13.5703125" collapsed="true"/>
+    <col min="10" max="16384" style="9" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="4" customFormat="1">
@@ -14520,7 +14533,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H4"/>
+  <dimension ref="B1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
@@ -14528,12 +14541,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="21.140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="16.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="21.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="16.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8">
@@ -14605,8 +14618,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="64.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="64.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="21.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23">
@@ -14617,7 +14630,7 @@
         <v>1750</v>
       </c>
     </row>
-    <row r="2" spans="1:23">
+    <row r="2">
       <c r="D2" t="s">
         <v>1751</v>
       </c>
@@ -15008,13 +15021,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="14" collapsed="1"/>
-    <col min="3" max="3" width="13.140625" style="14" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25" style="14" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.85546875" style="14" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.140625" style="14" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="33.5703125" style="14" customWidth="1" collapsed="1"/>
-    <col min="8" max="16384" width="9.140625" style="14" collapsed="1"/>
+    <col min="1" max="2" style="14" width="9.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="14" width="13.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="14" width="25.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="14" width="17.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="14" width="24.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="14" width="33.5703125" collapsed="true"/>
+    <col min="8" max="16384" style="14" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="45">
@@ -15114,13 +15127,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="16.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="13.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="30">
@@ -15267,14 +15280,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1">
       <c r="C1" t="s">
-        <v>1798</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>1806</v>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="s">
-        <v>1797</v>
+        <v>1805</v>
       </c>
     </row>
     <row r="4" spans="1:3">

</xml_diff>